<commit_message>
Set up the database
</commit_message>
<xml_diff>
--- a/tables/Listings.xlsx
+++ b/tables/Listings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanhaley/collab/Proj3collab/Data-607-Project-Three/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645950BE-CD01-2A4A-9891-9A2B0F127FF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E8D3F-8014-C04F-B5A4-6A39B09C385C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{02CBC0C0-4839-3F44-9571-173514640FF4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="187">
   <si>
     <t>Company</t>
   </si>
@@ -87,30 +87,15 @@
     <t>Degree</t>
   </si>
   <si>
-    <t>(P,R,J,C,ML,NL,ST,M, SQ,DW,NP,SC, PD, SK,PT,CF,TF,K,TH,TS)</t>
-  </si>
-  <si>
-    <t>(communicating)</t>
-  </si>
-  <si>
-    <t>(OO,C,DL,PB)</t>
-  </si>
-  <si>
     <t>Apple</t>
   </si>
   <si>
     <t>Data Scientist</t>
   </si>
   <si>
-    <t>(FT, SQ,R,TB,DA,ML,ST,SP,HP)</t>
-  </si>
-  <si>
     <t>Millennium</t>
   </si>
   <si>
-    <t>(DA, FT,P,C,J,SQ,)</t>
-  </si>
-  <si>
     <t>Plaid</t>
   </si>
   <si>
@@ -120,39 +105,15 @@
     <t>San Francisco</t>
   </si>
   <si>
-    <t>(models)</t>
-  </si>
-  <si>
-    <t>(analytics, business, presenting, communicating)</t>
-  </si>
-  <si>
-    <t>(FT,LD,ML,P,SP,DA)</t>
-  </si>
-  <si>
     <t>Uber</t>
   </si>
   <si>
-    <t>(DA,SQ,R,P,ST)</t>
-  </si>
-  <si>
-    <t>(research, economics, presenting, communicating)</t>
-  </si>
-  <si>
     <t>Fremont</t>
   </si>
   <si>
-    <t>(analytics, metrics)</t>
-  </si>
-  <si>
-    <t>(R,TB,P,SQ,V,NP,SC,PD,SK,ST,LD,DA,DW)</t>
-  </si>
-  <si>
     <t>Spotify</t>
   </si>
   <si>
-    <t>(DA,LD,FT,DW,SQ,P,PD,TB,BQ,V)</t>
-  </si>
-  <si>
     <t>Colgate</t>
   </si>
   <si>
@@ -162,27 +123,12 @@
     <t>NJ</t>
   </si>
   <si>
-    <t>(V)</t>
-  </si>
-  <si>
-    <t>(V,ST,P,TB)</t>
-  </si>
-  <si>
-    <t>(independent, communicating)</t>
-  </si>
-  <si>
     <t>Microsoft</t>
   </si>
   <si>
     <t xml:space="preserve">Data &amp; Applied Scientist </t>
   </si>
   <si>
-    <t>(ML,DL,P,NL,CV,TS,J,C)</t>
-  </si>
-  <si>
-    <t>(NP,PD,SK,R,G,TF,PT,SP,SQ,)</t>
-  </si>
-  <si>
     <t>Amazon</t>
   </si>
   <si>
@@ -192,27 +138,12 @@
     <t>VA</t>
   </si>
   <si>
-    <t>(ML,DL,LD,AWS,DL,CF,TF,TH,K)</t>
-  </si>
-  <si>
-    <t>(PB,J,C,P,R,SP,SK,SQ)</t>
-  </si>
-  <si>
-    <t>(presenting, communicating, business)</t>
-  </si>
-  <si>
     <t>Tiktok</t>
   </si>
   <si>
     <t>Mountain View</t>
   </si>
   <si>
-    <t>(SQ,P,LD,HP,ST)</t>
-  </si>
-  <si>
-    <t>(communicating, presenting)</t>
-  </si>
-  <si>
     <t>Aon</t>
   </si>
   <si>
@@ -225,66 +156,24 @@
     <t>WA</t>
   </si>
   <si>
-    <t>(P,R,MA,DA,ST,NP,PD,SK,SQ,M,)</t>
-  </si>
-  <si>
-    <t>(OO,P,M)</t>
-  </si>
-  <si>
-    <t>(metrics, communicating, models, logistics)</t>
-  </si>
-  <si>
-    <t>(DB)</t>
-  </si>
-  <si>
     <t>PlayStation</t>
   </si>
   <si>
     <t>San Mateo</t>
   </si>
   <si>
-    <t>(LD,SQ,P,R,DA)</t>
-  </si>
-  <si>
     <t>Adobe</t>
   </si>
   <si>
-    <t>(analytics, business, models)</t>
-  </si>
-  <si>
-    <t>(DA,ST,SQ,TB,P,R,TB,V)</t>
-  </si>
-  <si>
     <t>Phoenix Group</t>
   </si>
   <si>
-    <t>(DA,P,ST,SQ,SK,ML)</t>
-  </si>
-  <si>
-    <t>(models, analytics, business)</t>
-  </si>
-  <si>
     <t>Pepsi</t>
   </si>
   <si>
     <t>eCom Data Scientist</t>
   </si>
   <si>
-    <t>(business, communicating,)</t>
-  </si>
-  <si>
-    <t>(communicating, models,)</t>
-  </si>
-  <si>
-    <t>(business, communicating)</t>
-  </si>
-  <si>
-    <t>(ML,DA,NP,PD,SQ,AWS,M.ST)</t>
-  </si>
-  <si>
-    <t>(DL,SK)</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -306,27 +195,12 @@
     <t>Remote</t>
   </si>
   <si>
-    <t>(DA,DB,ST,R,P,SQ)</t>
-  </si>
-  <si>
-    <t>(SP,ML,DL,TF,K,)</t>
-  </si>
-  <si>
-    <t>(team, cloud, models)</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
     <t>Entry</t>
   </si>
   <si>
-    <t>(communicating, diversity, team)</t>
-  </si>
-  <si>
-    <t>(SQ,R,P,DA)</t>
-  </si>
-  <si>
     <t>Quora</t>
   </si>
   <si>
@@ -336,78 +210,33 @@
     <t>Senior</t>
   </si>
   <si>
-    <t>(metrics, models, communicating,</t>
-  </si>
-  <si>
-    <t>(V,ST,P,TB,P,R,DW,DA)</t>
-  </si>
-  <si>
-    <t>(LD,G)</t>
-  </si>
-  <si>
     <t>NASA</t>
   </si>
   <si>
     <t>Pasadena</t>
   </si>
   <si>
-    <t>(DA,ML,CV,C,P,J)</t>
-  </si>
-  <si>
-    <t>(communicating, AI, automation, team)</t>
-  </si>
-  <si>
     <t>Bluecore</t>
   </si>
   <si>
-    <t>(M,BQ,SP,SQ,K,TF,AF,KB,NN,ML,ST,M,DL,NL,TS)</t>
-  </si>
-  <si>
-    <t>(marketing, team )</t>
-  </si>
-  <si>
     <t>Snowflake</t>
   </si>
   <si>
-    <t>(TS,SQ,P,R,SK,TF,MA,ML,ST)</t>
-  </si>
-  <si>
-    <t>(cloud, security, communicating)</t>
-  </si>
-  <si>
     <t>Lyft</t>
   </si>
   <si>
     <t xml:space="preserve">Staff Data Scientist </t>
   </si>
   <si>
-    <t>(algorithms, communicating, business)</t>
-  </si>
-  <si>
-    <t>(DA,ST,ML,M,V,P,R,MA)</t>
-  </si>
-  <si>
     <t>Wish</t>
   </si>
   <si>
-    <t>(P,SQ,TB,V,UL,DA)</t>
-  </si>
-  <si>
     <t>Everlane</t>
   </si>
   <si>
-    <t>(SQ,ST,R,P,AWS)</t>
-  </si>
-  <si>
-    <t>(logistics, models)</t>
-  </si>
-  <si>
     <t>BlackRock</t>
   </si>
   <si>
-    <t>(ML,ST,DA,NL,V,NG,DB,TS,M,P,R,MA)</t>
-  </si>
-  <si>
     <t>Fidelity</t>
   </si>
   <si>
@@ -423,48 +252,18 @@
     <t>Director</t>
   </si>
   <si>
-    <t>(ML,DA,MA,R,ST,P,LD,V)</t>
-  </si>
-  <si>
     <t>Instagram</t>
   </si>
   <si>
-    <t>(DA,ST)</t>
-  </si>
-  <si>
-    <t>(HV,R,P)</t>
-  </si>
-  <si>
-    <t>(metrics, communicating, business, presenting, team)</t>
-  </si>
-  <si>
     <t>Moveworks</t>
   </si>
   <si>
-    <t>(product, AI, metrics, presenting, communicating, collaborate)</t>
-  </si>
-  <si>
-    <t>(SQ,P,V,DB,AWS,G)</t>
-  </si>
-  <si>
     <t>Pinterest</t>
   </si>
   <si>
-    <t>(forecasting, models)</t>
-  </si>
-  <si>
-    <t>(TS,ML,PT,TF,P,R)</t>
-  </si>
-  <si>
     <t>QuantumBlack</t>
   </si>
   <si>
-    <t>(ST,ML,R,P,SQ,SL,M)</t>
-  </si>
-  <si>
-    <t>(presenting, communicating, collaborate)</t>
-  </si>
-  <si>
     <t>Boston</t>
   </si>
   <si>
@@ -474,45 +273,21 @@
     <t>Happify Health</t>
   </si>
   <si>
-    <t>(NL,DL,ML,ST,P,TF,PT,TH,K,SK)</t>
-  </si>
-  <si>
-    <t>(AI, alogorithms, models)</t>
-  </si>
-  <si>
     <t>Gusto</t>
   </si>
   <si>
     <t>Principal</t>
   </si>
   <si>
-    <t>(product, analytics, collaborate, communicating)</t>
-  </si>
-  <si>
-    <t>(SQ,P,R,ST)</t>
-  </si>
-  <si>
     <t>Verizon</t>
   </si>
   <si>
     <t>Sunnyvale</t>
   </si>
   <si>
-    <t>(marketing, analytics, metrics, models, business, communicating, presenting)</t>
-  </si>
-  <si>
-    <t>(LD,SQ,P,R,DA,HV,HP,SP,ML,NN)</t>
-  </si>
-  <si>
     <t>Next Insurance</t>
   </si>
   <si>
-    <t>(analytics, metrics, quantitative,</t>
-  </si>
-  <si>
-    <t>(SQ,P,V)</t>
-  </si>
-  <si>
     <t>Palo Alto</t>
   </si>
   <si>
@@ -522,21 +297,9 @@
     <t>Splunk</t>
   </si>
   <si>
-    <t>(models, communicating, collaborate)</t>
-  </si>
-  <si>
-    <t>(DA,V,SE,LD)</t>
-  </si>
-  <si>
     <t>Outreach</t>
   </si>
   <si>
-    <t>(product, analytics, presenting, communicating, metrics</t>
-  </si>
-  <si>
-    <t>(SQ,V,P,SP,ST)</t>
-  </si>
-  <si>
     <t>Github</t>
   </si>
   <si>
@@ -549,12 +312,6 @@
     <t>UT</t>
   </si>
   <si>
-    <t>(SE,P,SQ,AWS,ML,M,ST)</t>
-  </si>
-  <si>
-    <t>(communicating, collaborate)</t>
-  </si>
-  <si>
     <t>Target</t>
   </si>
   <si>
@@ -567,18 +324,9 @@
     <t>MN</t>
   </si>
   <si>
-    <t>(DA,R,P,SQ,SL,M,ST,ML)</t>
-  </si>
-  <si>
-    <t>(collaborate)</t>
-  </si>
-  <si>
     <t>General Mills</t>
   </si>
   <si>
-    <t>(collaborate, models, marketing, analytics, cloud)</t>
-  </si>
-  <si>
     <t>Nielsen</t>
   </si>
   <si>
@@ -588,16 +336,265 @@
     <t>IL</t>
   </si>
   <si>
-    <t>(ST,SK,SP,SQ,AZ,AWS)</t>
-  </si>
-  <si>
-    <t>(quantitative, research, models, presenting, alternative data)</t>
-  </si>
-  <si>
-    <t>(digital, cloud, research)</t>
-  </si>
-  <si>
-    <t>(HP,SP,V,TB,R)</t>
+    <t>P,R,J,C,ML,NL,ST,M, SQ,DW,NP,SC, PD, SK,PT,CF,TF,K,TH,TS</t>
+  </si>
+  <si>
+    <t>FT,LD,ML,P,SP,DA</t>
+  </si>
+  <si>
+    <t>DA,SQ,R,P,ST</t>
+  </si>
+  <si>
+    <t>R,TB,P,SQ,V,NP,SC,PD,SK,ST,LD,DA,DW</t>
+  </si>
+  <si>
+    <t>DA,LD,FT,DW,SQ,P,PD,TB,BQ,V</t>
+  </si>
+  <si>
+    <t>V,ST,P,TB</t>
+  </si>
+  <si>
+    <t>ML,DL,P,NL,CV,TS,J,C</t>
+  </si>
+  <si>
+    <t>ML,DL,LD,AWS,DL,CF,TF,TH,K</t>
+  </si>
+  <si>
+    <t>SQ,P,LD,HP,ST</t>
+  </si>
+  <si>
+    <t>P,R,MA,DA,ST,NP,PD,SK,SQ,M</t>
+  </si>
+  <si>
+    <t>OO,P,M</t>
+  </si>
+  <si>
+    <t>LD,SQ,P,R,DA</t>
+  </si>
+  <si>
+    <t>DA,ST,SQ,TB,P,R,TB,V</t>
+  </si>
+  <si>
+    <t>DA,P,ST,SQ,SK,ML</t>
+  </si>
+  <si>
+    <t>ML,DA,NP,PD,SQ,AWS,M,ST</t>
+  </si>
+  <si>
+    <t>SQ,R,P,DA</t>
+  </si>
+  <si>
+    <t>V,ST,P,TB,P,R,DW,DA</t>
+  </si>
+  <si>
+    <t>DA,ML,CV,C,P,J</t>
+  </si>
+  <si>
+    <t>M,BQ,SP,SQ,K,TF,AF,KB,NN,ML,ST,M,DL,NL,TS</t>
+  </si>
+  <si>
+    <t>TS,SQ,P,R,SK,TF,MA,ML,ST</t>
+  </si>
+  <si>
+    <t>DA,ST,ML,M,V,P,R,MA</t>
+  </si>
+  <si>
+    <t>P,SQ,TB,V,UL,DA</t>
+  </si>
+  <si>
+    <t>SQ,ST,R,P,AWS</t>
+  </si>
+  <si>
+    <t>ML,ST,DA,NL,V,NG,DB,TS,M,P,R,MA</t>
+  </si>
+  <si>
+    <t>ML,DA,MA,R,ST,P,LD,V</t>
+  </si>
+  <si>
+    <t>DA,ST</t>
+  </si>
+  <si>
+    <t>SQ,P,V,DB,AWS,G</t>
+  </si>
+  <si>
+    <t>TS,ML,PT,TF,P,R</t>
+  </si>
+  <si>
+    <t>ST,ML,R,P,SQ,SL,M</t>
+  </si>
+  <si>
+    <t>NL,DL,ML,ST,P,TF,PT,TH,K,SK</t>
+  </si>
+  <si>
+    <t>SQ,P,R,ST</t>
+  </si>
+  <si>
+    <t>LD,SQ,P,R,DA,HV,HP,SP,ML,NN</t>
+  </si>
+  <si>
+    <t>SQ,P,V</t>
+  </si>
+  <si>
+    <t>DA,V,SE,LD</t>
+  </si>
+  <si>
+    <t>SQ,V,P,SP,ST</t>
+  </si>
+  <si>
+    <t>SE,P,SQ,AWS,ML,M,ST</t>
+  </si>
+  <si>
+    <t>DA,R,P,SQ,SL,M,ST,ML</t>
+  </si>
+  <si>
+    <t>HP,SP,V,TB,R</t>
+  </si>
+  <si>
+    <t>ST,SK,SP,SQ,AZ,AWS</t>
+  </si>
+  <si>
+    <t>HV,R,P</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>LD,G</t>
+  </si>
+  <si>
+    <t>SP,ML,DL,TF,K</t>
+  </si>
+  <si>
+    <t>DL,SK</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>PB,J,C,P,R,SP,SK,SQ</t>
+  </si>
+  <si>
+    <t>NP,PD,SK,R,G,TF,PT,SP,SQ</t>
+  </si>
+  <si>
+    <t>OO,C,DL,PB</t>
+  </si>
+  <si>
+    <t>communicating</t>
+  </si>
+  <si>
+    <t>analytics, business, presenting, communicating</t>
+  </si>
+  <si>
+    <t>models</t>
+  </si>
+  <si>
+    <t>research, economics, presenting, communicating</t>
+  </si>
+  <si>
+    <t>analytics, metrics</t>
+  </si>
+  <si>
+    <t>independent, communicating</t>
+  </si>
+  <si>
+    <t>communicating, models</t>
+  </si>
+  <si>
+    <t>presenting, communicating, business</t>
+  </si>
+  <si>
+    <t>communicating, presenting</t>
+  </si>
+  <si>
+    <t>metrics, communicating, models, logistics</t>
+  </si>
+  <si>
+    <t>business, communicating</t>
+  </si>
+  <si>
+    <t>analytics, business, models</t>
+  </si>
+  <si>
+    <t>models, analytics, business</t>
+  </si>
+  <si>
+    <t>team, cloud, models</t>
+  </si>
+  <si>
+    <t>communicating, diversity, team</t>
+  </si>
+  <si>
+    <t>metrics, models, communicating</t>
+  </si>
+  <si>
+    <t>communicating, AI, automation, team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marketing, team </t>
+  </si>
+  <si>
+    <t>cloud, security, communicating</t>
+  </si>
+  <si>
+    <t>algorithms, communicating, business</t>
+  </si>
+  <si>
+    <t>logistics, models</t>
+  </si>
+  <si>
+    <t>quantitative, research, models, presenting, alternative data</t>
+  </si>
+  <si>
+    <t>metrics, communicating, business, presenting, team</t>
+  </si>
+  <si>
+    <t>product, AI, metrics, presenting, communicating, collaborate</t>
+  </si>
+  <si>
+    <t>forecasting, models</t>
+  </si>
+  <si>
+    <t>presenting, communicating, collaborate</t>
+  </si>
+  <si>
+    <t>AI, alogorithms, models</t>
+  </si>
+  <si>
+    <t>product, analytics, collaborate, communicating</t>
+  </si>
+  <si>
+    <t>marketing, analytics, metrics, models, business, communicating, presenting</t>
+  </si>
+  <si>
+    <t>analytics, metrics, quantitative</t>
+  </si>
+  <si>
+    <t>models, communicating, collaborate</t>
+  </si>
+  <si>
+    <t>product, analytics, presenting, communicating, metrics</t>
+  </si>
+  <si>
+    <t>communicating, collaborate</t>
+  </si>
+  <si>
+    <t>collaborate</t>
+  </si>
+  <si>
+    <t>collaborate, models, marketing, analytics, cloud</t>
+  </si>
+  <si>
+    <t>digital, cloud, research</t>
+  </si>
+  <si>
+    <t>DA,DB,ST,R,P,SQ</t>
+  </si>
+  <si>
+    <t>DA,FT,P,C,J,SQ</t>
+  </si>
+  <si>
+    <t>FT,SQ,R,TB,DA,ML,ST,SP,HP</t>
   </si>
 </sst>
 </file>
@@ -951,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D97821E-F653-FE48-999D-8EE7A536F327}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,10 +1004,10 @@
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1045,13 +1042,13 @@
         <v>178</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="N2">
         <v>10000</v>
@@ -1059,10 +1056,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -1089,13 +1086,13 @@
         <v>191</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>186</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>186</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>149</v>
       </c>
       <c r="N3">
         <v>10000</v>
@@ -1103,10 +1100,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1133,13 +1130,13 @@
         <v>203</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>185</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="N4">
         <v>1000</v>
@@ -1147,10 +1144,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -1165,10 +1162,10 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I5">
         <v>102</v>
@@ -1177,27 +1174,27 @@
         <v>224</v>
       </c>
       <c r="K5" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="N5">
         <v>250</v>
       </c>
       <c r="O5" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1212,10 +1209,10 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>110</v>
@@ -1224,13 +1221,13 @@
         <v>168</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>151</v>
       </c>
       <c r="N6">
         <v>10000</v>
@@ -1241,7 +1238,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1256,10 +1253,10 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I7">
         <v>115</v>
@@ -1268,13 +1265,13 @@
         <v>190</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="L7" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="N7">
         <v>10000</v>
@@ -1282,10 +1279,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1312,13 +1309,13 @@
         <v>154</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="N8">
         <v>10000</v>
@@ -1326,10 +1323,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -1344,10 +1341,10 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1356,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="N9">
         <v>10000</v>
@@ -1370,10 +1367,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1388,10 +1385,10 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1400,13 +1397,13 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>146</v>
       </c>
       <c r="M10" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="N10">
         <v>10000</v>
@@ -1414,10 +1411,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1432,10 +1429,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="I11">
         <v>101</v>
@@ -1444,13 +1441,13 @@
         <v>179</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="L11" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="M11" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="N11">
         <v>10000</v>
@@ -1458,10 +1455,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1476,10 +1473,10 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I12">
         <v>106</v>
@@ -1488,27 +1485,27 @@
         <v>231</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="M12" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="N12">
         <v>5000</v>
       </c>
       <c r="O12" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1523,10 +1520,10 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1535,27 +1532,27 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="M13" t="s">
-        <v>18</v>
+        <v>148</v>
       </c>
       <c r="N13">
         <v>10000</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1570,10 +1567,10 @@
         <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I14">
         <v>110</v>
@@ -1582,13 +1579,13 @@
         <v>150</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>157</v>
       </c>
       <c r="N14">
         <v>10000</v>
@@ -1596,10 +1593,10 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1614,10 +1611,10 @@
         <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I15">
         <v>103</v>
@@ -1626,13 +1623,13 @@
         <v>219</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="M15" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="N15">
         <v>5000</v>
@@ -1640,10 +1637,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1658,10 +1655,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I16">
         <v>112</v>
@@ -1670,27 +1667,27 @@
         <v>197</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="M16" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="N16">
         <v>10000</v>
       </c>
       <c r="O16" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -1717,27 +1714,27 @@
         <v>150</v>
       </c>
       <c r="K17" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="M17" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1764,27 +1761,27 @@
         <v>165</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="L18" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="M18" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="N18">
         <v>10000</v>
       </c>
       <c r="O18" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1799,10 +1796,10 @@
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1811,46 +1808,46 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>184</v>
       </c>
       <c r="L19" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="M19" t="s">
-        <v>92</v>
+        <v>161</v>
       </c>
       <c r="N19">
         <v>10000</v>
       </c>
       <c r="O19" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
         <v>21</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
       <c r="I20">
         <v>0</v>
       </c>
@@ -1858,27 +1855,27 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="M20" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -1893,10 +1890,10 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1905,27 +1902,27 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="L21" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="M21" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="N21">
         <v>250</v>
       </c>
       <c r="O21" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1940,10 +1937,10 @@
         <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="H22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I22">
         <v>92</v>
@@ -1952,27 +1949,27 @@
         <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="L22" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="N22">
         <v>5000</v>
       </c>
       <c r="O22" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1999,27 +1996,27 @@
         <v>145</v>
       </c>
       <c r="K23" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="L23" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="M23" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -2034,10 +2031,10 @@
         <v>5</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="H24" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I24">
         <v>128</v>
@@ -2046,27 +2043,27 @@
         <v>216</v>
       </c>
       <c r="K24" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="M24" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="N24">
         <v>1000</v>
       </c>
       <c r="O24" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="C25">
         <v>6</v>
@@ -2081,10 +2078,10 @@
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I25">
         <v>125</v>
@@ -2093,27 +2090,27 @@
         <v>194</v>
       </c>
       <c r="K25" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L25" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="M25" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="N25">
         <v>5000</v>
       </c>
       <c r="O25" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2128,10 +2125,10 @@
         <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I26">
         <v>125</v>
@@ -2140,27 +2137,27 @@
         <v>224</v>
       </c>
       <c r="K26" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="L26" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M26" t="s">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="N26">
         <v>500</v>
       </c>
       <c r="O26" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -2175,10 +2172,10 @@
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I27">
         <v>113</v>
@@ -2187,27 +2184,27 @@
         <v>191</v>
       </c>
       <c r="K27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="L27" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="M27" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -2240,7 +2237,7 @@
         <v>123</v>
       </c>
       <c r="M28" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="N28">
         <v>10000</v>
@@ -2248,10 +2245,10 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -2266,10 +2263,10 @@
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>127</v>
+        <v>70</v>
       </c>
       <c r="I29">
         <v>100</v>
@@ -2278,27 +2275,27 @@
         <v>156</v>
       </c>
       <c r="K29" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L29" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="M29" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="N29">
         <v>10000</v>
       </c>
       <c r="O29" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -2313,10 +2310,10 @@
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I30">
         <v>87</v>
@@ -2325,13 +2322,13 @@
         <v>209</v>
       </c>
       <c r="K30" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="L30" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="M30" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="N30">
         <v>10000</v>
@@ -2339,10 +2336,10 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -2357,10 +2354,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H31" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I31">
         <v>99</v>
@@ -2369,27 +2366,27 @@
         <v>215</v>
       </c>
       <c r="K31" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="L31" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="M31" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="C32">
         <v>5</v>
@@ -2404,10 +2401,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H32" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I32">
         <v>120</v>
@@ -2416,27 +2413,27 @@
         <v>230</v>
       </c>
       <c r="K32" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="L32" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="M32" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="N32">
         <v>1000</v>
       </c>
       <c r="O32" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2451,10 +2448,10 @@
         <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="H33" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="I33">
         <v>86</v>
@@ -2463,27 +2460,27 @@
         <v>187</v>
       </c>
       <c r="K33" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="L33" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="M33" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="N33">
         <v>250</v>
       </c>
       <c r="O33" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2510,27 +2507,27 @@
         <v>186</v>
       </c>
       <c r="K34" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="L34" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="M34" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="N34">
         <v>25</v>
       </c>
       <c r="O34" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -2557,27 +2554,27 @@
         <v>189</v>
       </c>
       <c r="K35" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="L35" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="M35" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="N35">
         <v>1000</v>
       </c>
       <c r="O35" t="s">
-        <v>149</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2592,10 +2589,10 @@
         <v>3</v>
       </c>
       <c r="G36" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="H36" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I36">
         <v>117</v>
@@ -2604,45 +2601,45 @@
         <v>196</v>
       </c>
       <c r="K36" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="L36" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="M36" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="N36">
         <v>10000</v>
       </c>
       <c r="O36" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>84</v>
+      </c>
+      <c r="H37" t="s">
         <v>21</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37" t="s">
-        <v>159</v>
-      </c>
-      <c r="H37" t="s">
-        <v>26</v>
       </c>
       <c r="I37">
         <v>100</v>
@@ -2651,27 +2648,27 @@
         <v>219</v>
       </c>
       <c r="K37" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="L37" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="M37" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="N37">
         <v>250</v>
       </c>
       <c r="O37" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2686,10 +2683,10 @@
         <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H38" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I38">
         <v>129</v>
@@ -2698,13 +2695,13 @@
         <v>203</v>
       </c>
       <c r="K38" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="L38" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="M38" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="N38">
         <v>5000</v>
@@ -2712,10 +2709,10 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -2730,10 +2727,10 @@
         <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="H39" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I39">
         <v>114</v>
@@ -2742,27 +2739,27 @@
         <v>179</v>
       </c>
       <c r="K39" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="L39" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="M39" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="N39">
         <v>500</v>
       </c>
       <c r="O39" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -2777,10 +2774,10 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>169</v>
+        <v>90</v>
       </c>
       <c r="H40" t="s">
-        <v>170</v>
+        <v>91</v>
       </c>
       <c r="I40">
         <v>114</v>
@@ -2789,27 +2786,27 @@
         <v>203</v>
       </c>
       <c r="K40" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="L40" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="M40" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="N40">
         <v>500</v>
       </c>
       <c r="O40" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>173</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -2824,10 +2821,10 @@
         <v>2</v>
       </c>
       <c r="G41" t="s">
-        <v>175</v>
+        <v>94</v>
       </c>
       <c r="H41" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="I41">
         <v>98</v>
@@ -2836,27 +2833,27 @@
         <v>198</v>
       </c>
       <c r="K41" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="L41" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="M41" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N41">
         <v>10000</v>
       </c>
       <c r="O41" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>93</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -2871,10 +2868,10 @@
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>175</v>
+        <v>94</v>
       </c>
       <c r="H42" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="I42">
         <v>122</v>
@@ -2883,27 +2880,27 @@
         <v>214</v>
       </c>
       <c r="K42" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="L42" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="M42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="N42">
         <v>10000</v>
       </c>
       <c r="O42" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>89</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -2918,10 +2915,10 @@
         <v>3</v>
       </c>
       <c r="G43" t="s">
-        <v>182</v>
+        <v>98</v>
       </c>
       <c r="H43" t="s">
-        <v>183</v>
+        <v>99</v>
       </c>
       <c r="I43">
         <v>77</v>
@@ -2930,13 +2927,13 @@
         <v>143</v>
       </c>
       <c r="K43" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="L43" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="M43" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N43">
         <v>10000</v>

</xml_diff>